<commit_message>
Picture In Picture Capability Added
</commit_message>
<xml_diff>
--- a/Output/Updated Excel/27_06_21_Consolidated.xlsx
+++ b/Output/Updated Excel/27_06_21_Consolidated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saura\Documents\UiPath\UiPathDemo\Output\Processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AA4CE7-B022-4E1D-8D3B-AA61E27739A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1500F2-A658-4E11-B147-36FDF5C8E745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -433,7 +433,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>